<commit_message>
Auto export CCCTR-1111 - test
</commit_message>
<xml_diff>
--- a/exports/testcases_CCCTR-1111_-_test.xlsx
+++ b/exports/testcases_CCCTR-1111_-_test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:M65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,20 +486,15 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Step #</t>
+          <t>Step Name (Design Steps)</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Step Name (Design Steps)</t>
+          <t>Description (Design Steps)</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Description (Design Steps)</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Expected (Design Steps)</t>
         </is>
@@ -558,20 +553,17 @@
           <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il</t>
         </is>
       </c>
-      <c r="K2" t="n">
-        <v>1</v>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il_STEP1</t>
+          <t>U zakaznika jdi na sluzby a zaloz objednavku na aktivaci pevneho internetu z roletky</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
-        <is>
-          <t>U zakaznika jdi na sluzby a zaloz objednavku na aktivaci pevneho internetu z roletky</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
         <is>
           <t>Prokliknuti do kosiku</t>
         </is>
@@ -630,20 +622,17 @@
           <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il</t>
         </is>
       </c>
-      <c r="K3" t="n">
-        <v>2</v>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il_STEP2</t>
+          <t xml:space="preserve">Vyber, ze zakaznik nemá pripojku a pokracuj na vyhledani podle adresy  </t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Vyber, ze zakaznik nemá pripojku a pokracuj na vyhledani podle adresy  </t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
         <is>
           <t>Otevre se vyhledavani dostupnosti podle adresy</t>
         </is>
@@ -702,20 +691,17 @@
           <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il</t>
         </is>
       </c>
-      <c r="K4" t="n">
-        <v>3</v>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il_STEP3</t>
+          <t xml:space="preserve">Over adresu na webu a zadej RUIAN nebo primo adresu, pokracovat </t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Over adresu na webu a zadej RUIAN nebo primo adresu, pokracovat </t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
         <is>
           <t>Adresa je dostupna s pozadovanou technologii, prokliknuti na další stranu uspesne</t>
         </is>
@@ -774,20 +760,17 @@
           <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il</t>
         </is>
       </c>
-      <c r="K5" t="n">
-        <v>4</v>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il_STEP4</t>
+          <t>Upresneni instalacni adresy potvrd pokracovat</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
-        <is>
-          <t>Upresneni instalacni adresy potvrd pokracovat</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
         <is>
           <t>Propsana adresa, prokliknuti na další stranu</t>
         </is>
@@ -846,20 +829,17 @@
           <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il</t>
         </is>
       </c>
-      <c r="K6" t="n">
-        <v>5</v>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il_STEP5</t>
+          <t>Z dostupne nabidky vyber pozadovany tarif, dej pokracovat a na další strane potvrd aktivacni balicek tehoz tarifu</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
-        <is>
-          <t>Z dostupne nabidky vyber pozadovany tarif, dej pokracovat a na další strane potvrd aktivacni balicek tehoz tarifu</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
         <is>
           <t>Vybran pozadovany tarif, prokliknuti na další stranu</t>
         </is>
@@ -918,20 +898,17 @@
           <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il</t>
         </is>
       </c>
-      <c r="K7" t="n">
-        <v>6</v>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il_STEP6</t>
+          <t>Preskoc vyber TV tarifu</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
-        <is>
-          <t>Preskoc vyber TV tarifu</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
         <is>
           <t>Zobrazeni další stranky</t>
         </is>
@@ -990,20 +967,17 @@
           <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il</t>
         </is>
       </c>
-      <c r="K8" t="n">
-        <v>7</v>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il_STEP7</t>
+          <t>Proklikej se standardnim postupem k odeslani objednavky</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
-        <is>
-          <t>Proklikej se standardnim postupem k odeslani objednavky</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
         <is>
           <t>Zobrazeni stranky s vyberem Security</t>
         </is>
@@ -1062,20 +1036,17 @@
           <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il</t>
         </is>
       </c>
-      <c r="K9" t="n">
-        <v>8</v>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il_STEP8</t>
+          <t>Vyber balicek Security dle pozadavku</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
-        <is>
-          <t>Vyber balicek Security dle pozadavku</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
         <is>
           <t>Balicek Security pridan/nepridan do kosiku</t>
         </is>
@@ -1134,20 +1105,17 @@
           <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il</t>
         </is>
       </c>
-      <c r="K10" t="n">
-        <v>9</v>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il_STEP9</t>
+          <t>Vyber pozadovany HW, dej pokracovat a na další strane potvrd vybrany HW</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
-        <is>
-          <t>Vyber pozadovany HW, dej pokracovat a na další strane potvrd vybrany HW</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
         <is>
           <t>HW vybran a potvrzen</t>
         </is>
@@ -1206,20 +1174,17 @@
           <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il</t>
         </is>
       </c>
-      <c r="K11" t="n">
-        <v>10</v>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il_STEP10</t>
+          <t>Souhlas s pridanim do magenty a na další strance s vybranym HW</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
-        <is>
-          <t>Souhlas s pridanim do magenty a na další strance s vybranym HW</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
         <is>
           <t>Odsouhlasena magenta a vybrany HW</t>
         </is>
@@ -1278,20 +1243,17 @@
           <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il</t>
         </is>
       </c>
-      <c r="K12" t="n">
-        <v>11</v>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il_STEP11</t>
+          <t>Nech predzaskrtnuty Wi-fi Manager a pokracuj</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
-        <is>
-          <t>Nech predzaskrtnuty Wi-fi Manager a pokracuj</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
         <is>
           <t>Wi-fi Manager screena se zobrazi a jde pokracovat do kosiku</t>
         </is>
@@ -1350,20 +1312,17 @@
           <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il</t>
         </is>
       </c>
-      <c r="K13" t="n">
-        <v>12</v>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il_STEP12</t>
+          <t>Zobrazeni kosiku, kontrola pridanych polozek</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
-        <is>
-          <t>Zobrazeni kosiku, kontrola pridanych polozek</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
         <is>
           <t>Všechny polozky souhlasi, kosik se otevrel spravne</t>
         </is>
@@ -1422,20 +1381,17 @@
           <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il</t>
         </is>
       </c>
-      <c r="K14" t="n">
-        <v>13</v>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il_STEP13</t>
+          <t>Kliknout na odeslat objednavku</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
-        <is>
-          <t>Kliknout na odeslat objednavku</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
         <is>
           <t>Prokliknuti na potvrzeni udaju zakaznika</t>
         </is>
@@ -1494,20 +1450,17 @@
           <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il</t>
         </is>
       </c>
-      <c r="K15" t="n">
-        <v>14</v>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il_STEP14</t>
+          <t>U udaju zakaznika pokracuj az ke strance s dokumenty</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
-        <is>
-          <t>U udaju zakaznika pokracuj az ke strance s dokumenty</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
         <is>
           <t>Všechny udaje zadane, prokliknuti na zaverecnou stranku</t>
         </is>
@@ -1566,20 +1519,17 @@
           <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il</t>
         </is>
       </c>
-      <c r="K16" t="n">
-        <v>15</v>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il_STEP15</t>
+          <t>Vytiskni smlouvy, zkontroluj smlouvy a podepis pozadovanym zpusobem</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
-        <is>
-          <t>Vytiskni smlouvy, zkontroluj smlouvy a podepis pozadovanym zpusobem</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
         <is>
           <t>Smlouvy jdou vytisknout, udaje odpovidaji objednavka odeslana</t>
         </is>
@@ -1638,20 +1588,17 @@
           <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il</t>
         </is>
       </c>
-      <c r="K17" t="n">
-        <v>16</v>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il_STEP16</t>
+          <t>Objednavku odesli, v pripade penezni transakce ISS dokonci platbu</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
-        <is>
-          <t>Objednavku odesli, v pripade penezni transakce ISS dokonci platbu</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
         <is>
           <t>Objednavka odeslana</t>
         </is>
@@ -1710,20 +1657,17 @@
           <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il</t>
         </is>
       </c>
-      <c r="K18" t="n">
-        <v>17</v>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il_STEP17</t>
+          <t>U DSL odesli email na dokonceni objednavky od CETIN a nasledne vyskladni v SAP</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
-        <is>
-          <t>U DSL odesli email na dokonceni objednavky od CETIN a nasledne vyskladni v SAP</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
         <is>
           <t>CETIN ok</t>
         </is>
@@ -1782,20 +1726,17 @@
           <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il</t>
         </is>
       </c>
-      <c r="K19" t="n">
-        <v>18</v>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il_STEP18</t>
+          <t>Zaloz OT na kontrolu sluzby na OSS PE se zadanymi udaji z COM</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
-        <is>
-          <t>Zaloz OT na kontrolu sluzby na OSS PE se zadanymi udaji z COM</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
         <is>
           <t>OT zpracovano bez chyb</t>
         </is>
@@ -1854,20 +1795,17 @@
           <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il</t>
         </is>
       </c>
-      <c r="K20" t="n">
-        <v>19</v>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il_STEP19</t>
+          <t>Proved kontrolu dokoncene objednavky v Siebel a COM a zkontroluj aktivni atribut v designoss</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
-        <is>
-          <t>Proved kontrolu dokoncene objednavky v Siebel a COM a zkontroluj aktivni atribut v designoss</t>
-        </is>
-      </c>
-      <c r="N20" t="inlineStr">
         <is>
           <t>Objednavka je spravne dokoncena, atribut je aktivni: FWA/CFS 220_provider = 2; DSL/CFS 207_provider = 2; OPTIN/DNS profile = FIXCZNIC…</t>
         </is>
@@ -1926,20 +1864,17 @@
           <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il</t>
         </is>
       </c>
-      <c r="K21" t="n">
-        <v>20</v>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>001_IL_B2B_DSL_aktivuj_dsl_+_security_na_b2b_pres_il_STEP20</t>
+          <t>Proved kontrolu notifikaci SMS/Email</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
-        <is>
-          <t>Proved kontrolu notifikaci SMS/Email</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr">
         <is>
           <t>SMS/Email odpovida sablone</t>
         </is>
@@ -1985,7 +1920,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>1-High</t>
+          <t>2-Medium</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1995,23 +1930,20 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>002_IL_B2B_DSL_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il</t>
-        </is>
-      </c>
-      <c r="K22" t="n">
-        <v>1</v>
+          <t>002_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>002_IL_B2B_DSL_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il_STEP1</t>
+          <t>V Siebel jdi na objednavky mimo zakaznika, hromadne objednavky</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
-        <is>
-          <t>V Siebel jdi na objednavky mimo zakaznika, hromadne objednavky</t>
-        </is>
-      </c>
-      <c r="N22" t="inlineStr">
         <is>
           <t>Otevre se prehled hromadnych objednavek</t>
         </is>
@@ -2057,7 +1989,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1-High</t>
+          <t>2-Medium</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -2067,23 +1999,20 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>002_IL_B2B_DSL_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il</t>
-        </is>
-      </c>
-      <c r="K23" t="n">
-        <v>2</v>
+          <t>002_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>002_IL_B2B_DSL_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il_STEP2</t>
+          <t>V zalozce sablony objednavek vytvor novou sablonu dle pozadavku</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
-        <is>
-          <t>V zalozce sablony objednavek vytvor novou sablonu dle pozadavku</t>
-        </is>
-      </c>
-      <c r="N23" t="inlineStr">
         <is>
           <t>Vypsan typ, nazev a zalozena sablona</t>
         </is>
@@ -2129,7 +2058,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>1-High</t>
+          <t>2-Medium</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -2139,23 +2068,20 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>002_IL_B2B_DSL_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il</t>
-        </is>
-      </c>
-      <c r="K24" t="n">
-        <v>3</v>
+          <t>002_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>002_IL_B2B_DSL_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il_STEP3</t>
+          <t>Pred ulozenim sablony pridej polozku na pozadovany PO... typ pozadovane akce (nikdy nemichat vic polozek dohromady, muze vznikat duplikace)</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
-        <is>
-          <t>Pred ulozenim sablony pridej polozku na pozadovany PO... typ pozadovane akce (nikdy nemichat vic polozek dohromady, muze vznikat duplikace)</t>
-        </is>
-      </c>
-      <c r="N24" t="inlineStr">
         <is>
           <t>Polozka byla pridana</t>
         </is>
@@ -2201,7 +2127,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1-High</t>
+          <t>2-Medium</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -2211,23 +2137,20 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>002_IL_B2B_DSL_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il</t>
-        </is>
-      </c>
-      <c r="K25" t="n">
-        <v>4</v>
+          <t>002_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>002_IL_B2B_DSL_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il_STEP4</t>
+          <t>Sablonu nyni uloz a aktivuj, opis si jeji cislo</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
-        <is>
-          <t>Sablonu nyni uloz a aktivuj, opis si jeji cislo</t>
-        </is>
-      </c>
-      <c r="N25" t="inlineStr">
         <is>
           <t>Otevre se prehled sablon s nami vytvorenou novou sablonou</t>
         </is>
@@ -2273,7 +2196,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1-High</t>
+          <t>2-Medium</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -2283,23 +2206,20 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>002_IL_B2B_DSL_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il</t>
-        </is>
-      </c>
-      <c r="K26" t="n">
-        <v>5</v>
+          <t>002_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>002_IL_B2B_DSL_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il_STEP5</t>
+          <t>Prejdi na hromadne objednavky a klikni na nova hromadna objednavka</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
-        <is>
-          <t>Prejdi na hromadne objednavky a klikni na nova hromadna objednavka</t>
-        </is>
-      </c>
-      <c r="N26" t="inlineStr">
         <is>
           <t>Otevre se formular objednavky</t>
         </is>
@@ -2345,7 +2265,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1-High</t>
+          <t>2-Medium</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -2355,23 +2275,20 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>002_IL_B2B_DSL_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il</t>
-        </is>
-      </c>
-      <c r="K27" t="n">
-        <v>6</v>
+          <t>002_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>002_IL_B2B_DSL_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il_STEP6</t>
+          <t>Napis typ a nazev objednavky a pokracuj</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
-        <is>
-          <t>Napis typ a nazev objednavky a pokracuj</t>
-        </is>
-      </c>
-      <c r="N27" t="inlineStr">
         <is>
           <t>Otevre se objednavkovy formular</t>
         </is>
@@ -2417,7 +2334,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1-High</t>
+          <t>2-Medium</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2427,23 +2344,20 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>002_IL_B2B_DSL_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il</t>
-        </is>
-      </c>
-      <c r="K28" t="n">
-        <v>7</v>
+          <t>002_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>002_IL_B2B_DSL_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il_STEP7</t>
+          <t>Stahni soubor .xlxs a vypln pozadovane sloupce - 1. sloupec zkopirovane cislo sablony, cislo sluzby, notifikace</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
-        <is>
-          <t>Stahni soubor .xlxs a vypln pozadovane sloupce - 1. sloupec zkopirovane cislo sablony, cislo sluzby, notifikace</t>
-        </is>
-      </c>
-      <c r="N28" t="inlineStr">
         <is>
           <t>Soubor jde stahnout, je vyplneny ulozeny a znovu nahrany</t>
         </is>
@@ -2489,7 +2403,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1-High</t>
+          <t>2-Medium</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2499,23 +2413,20 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>002_IL_B2B_DSL_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il</t>
-        </is>
-      </c>
-      <c r="K29" t="n">
-        <v>8</v>
+          <t>002_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>002_IL_B2B_DSL_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il_STEP8</t>
+          <t>Po par vterinach klikni na aktualizovat stav a odeslat hromadnou objednavku</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
-        <is>
-          <t>Po par vterinach klikni na aktualizovat stav a odeslat hromadnou objednavku</t>
-        </is>
-      </c>
-      <c r="N29" t="inlineStr">
         <is>
           <t>Propsal se nahrany soubor a objednavka sla odeslat</t>
         </is>
@@ -2561,7 +2472,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1-High</t>
+          <t>2-Medium</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2571,23 +2482,20 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>002_IL_B2B_DSL_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il</t>
-        </is>
-      </c>
-      <c r="K30" t="n">
-        <v>9</v>
+          <t>002_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>002_IL_B2B_DSL_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il_STEP9</t>
+          <t>V COM/bulk orders zkontroluj prubeh obejdnavky</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
-        <is>
-          <t>V COM/bulk orders zkontroluj prubeh obejdnavky</t>
-        </is>
-      </c>
-      <c r="N30" t="inlineStr">
         <is>
           <t>Objednavka je completed a kladne dokoncena</t>
         </is>
@@ -2633,7 +2541,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>1-High</t>
+          <t>2-Medium</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2643,25 +2551,2368 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>002_IL_B2B_DSL_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il</t>
-        </is>
-      </c>
-      <c r="K31" t="n">
-        <v>10</v>
+          <t>002_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>002_IL_B2B_DSL_aktivuj_dsl_pomoci_bulk_na_b2b_pres_il_STEP10</t>
+          <t>V Siebel zkontroluj dokoncenou objednavku a provedene akce na sluzbe</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>V Siebel zkontroluj dokoncenou objednavku a provedene akce na sluzbe</t>
-        </is>
-      </c>
-      <c r="N31" t="inlineStr">
-        <is>
           <t>Objednavka je dokoncena a pozadovana akce se vydarila</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Aktivace + VAS - FIX</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>2-Huge</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>003_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>U zakaznika jdi na sluzby a zaloz objednavku na aktivaci pevneho internetu z roletky</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>Prokliknuti do kosiku</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Aktivace + VAS - FIX</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>2-Huge</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>003_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vyber, ze zakaznik nemá pripojku a pokracuj na vyhledani podle adresy  </t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>Otevre se vyhledavani dostupnosti podle adresy</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Aktivace + VAS - FIX</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>2-Huge</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>003_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Over adresu na webu a zadej RUIAN nebo primo adresu, pokracovat </t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>Adresa je dostupna s pozadovanou technologii, prokliknuti na další stranu uspesne</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Aktivace + VAS - FIX</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>2-Huge</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>003_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>Upresneni instalacni adresy potvrd pokracovat</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>Propsana adresa, prokliknuti na další stranu</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Aktivace + VAS - FIX</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>2-Huge</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>003_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>Z dostupne nabidky vyber pozadovany tarif, dej pokracovat a na další strane potvrd aktivacni balicek tehoz tarifu</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>Vybran pozadovany tarif, prokliknuti na další stranu</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Aktivace + VAS - FIX</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>2-Huge</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>003_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>Preskoc vyber TV tarifu</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>Zobrazeni další stranky</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Aktivace + VAS - FIX</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>2-Huge</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>003_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>Proklikej se standardnim postupem k odeslani objednavky</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>Zobrazeni stranky s vyberem Security</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Aktivace + VAS - FIX</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>2-Huge</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>003_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>Vyber balicek Security dle pozadavku</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>Balicek Security pridan/nepridan do kosiku</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Aktivace + VAS - FIX</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>2-Huge</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>003_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>Vyber pozadovany HW, dej pokracovat a na další strane potvrd vybrany HW</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>HW vybran a potvrzen</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Aktivace + VAS - FIX</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>2-Huge</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>003_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>Souhlas s pridanim do magenty a na další strance s vybranym HW</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>Odsouhlasena magenta a vybrany HW</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Aktivace + VAS - FIX</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>2-Huge</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>003_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>Nech predzaskrtnuty Wi-fi Manager a pokracuj</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>Wi-fi Manager screena se zobrazi a jde pokracovat do kosiku</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Aktivace + VAS - FIX</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>2-Huge</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>003_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>Zobrazeni kosiku, kontrola pridanych polozek</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>Všechny polozky souhlasi, kosik se otevrel spravne</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Aktivace + VAS - FIX</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>2-Huge</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>003_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>Kliknout na odeslat objednavku</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>Prokliknuti na potvrzeni udaju zakaznika</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Aktivace + VAS - FIX</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>2-Huge</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>003_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>U udaju zakaznika pokracuj az ke strance s dokumenty</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>Všechny udaje zadane, prokliknuti na zaverecnou stranku</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Aktivace + VAS - FIX</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>2-Huge</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>003_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Vytiskni smlouvy, zkontroluj smlouvy a podepis pozadovanym zpusobem</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>Smlouvy jdou vytisknout, udaje odpovidaji objednavka odeslana</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Aktivace + VAS - FIX</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>2-Huge</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>003_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>Objednavku odesli, v pripade penezni transakce ISS dokonci platbu</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>Objednavka odeslana</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Aktivace + VAS - FIX</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>2-Huge</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>003_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>U DSL odesli email na dokonceni objednavky od CETIN a nasledne vyskladni v SAP</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>CETIN ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Aktivace + VAS - FIX</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>2-Huge</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>003_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>Zaloz OT na kontrolu sluzby na OSS PE se zadanymi udaji z COM</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>OT zpracovano bez chyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Aktivace + VAS - FIX</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>2-Huge</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>003_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>Proved kontrolu dokoncene objednavky v Siebel a COM a zkontroluj aktivni atribut v designoss</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>Objednavka je spravne dokoncena, atribut je aktivni: FWA/CFS 220_provider = 2; DSL/CFS 207_provider = 2; OPTIN/DNS profile = FIXCZNIC…</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Aktivace + VAS - FIX</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>2-Huge</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>003_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>Proved kontrolu notifikaci SMS/Email</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>SMS/Email odpovida sablone</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Dokup VAS - HLAS</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>4-Medium</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>004_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>Vytvor si aktivni mobilni tarif Next bez Security a najed na ni ve sluzbach</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>Sluzba dle pozadavku aktivni</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Dokup VAS - HLAS</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>4-Medium</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>004_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>Klikni na objednat a dostan se do kosiku</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>Kosik otevreny</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Dokup VAS - HLAS</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>4-Medium</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>004_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>Vyhledej balicek dle pozadavku a pridej do kosiku</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>Balicek se zobrazi a jde pridat do kosiku</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Dokup VAS - HLAS</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>4-Medium</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>004_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>Zkontroluj pridani spravnych atributu do kosiku a dokonci objednavku</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>Atributy v kosiku OK, objednavka odeslana</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Dokup VAS - HLAS</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>4-Medium</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>004_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>V COM konzoli zkontroluj rozpad tasku a kladny prubeh objednavky</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>Prubeh objednavky OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Dokup VAS - HLAS</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>4-Medium</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>004_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>V Siebel zkontroluj, ze je objednavka dokoncena a u sluzby je aktivni balicek</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>Objednavka dokoncena, balicek je aktivni u sluzby</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Dokup VAS - HLAS</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>4-Medium</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>004_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>Proved kontrolu notifikaci SMS/Email</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>SMS/Email odpovida sablone</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Dokup VAS - HLAS</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>3-Big</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>005_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>Vytvor si aktivni mobilni tarif Next bez Security a najed na ni ve sluzbach</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>Sluzba dle pozadavku aktivni</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Dokup VAS - HLAS</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>3-Big</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>005_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>Klikni na objednat a dostan se do kosiku</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>Kosik otevreny</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Dokup VAS - HLAS</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>3-Big</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>005_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>Vyhledej balicek dle pozadavku a pridej do kosiku</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>Balicek se zobrazi a jde pridat do kosiku</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Dokup VAS - HLAS</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>3-Big</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>005_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>Zkontroluj pridani spravnych atributu do kosiku a dokonci objednavku</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>Atributy v kosiku OK, objednavka odeslana</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Dokup VAS - HLAS</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>3-Big</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>005_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>V COM konzoli zkontroluj rozpad tasku a kladny prubeh objednavky</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>Prubeh objednavky OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Dokup VAS - HLAS</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>3-Big</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>005_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>V Siebel zkontroluj, ze je objednavka dokoncena a u sluzby je aktivni balicek</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>Objednavka dokoncena, balicek je aktivni u sluzby</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>CCCTR-1111 - test</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>UAT2\Antosova\</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Siebel_CZ</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Segment: B2C
+Kanál: SHOP
+Akce: Dokup VAS - HLAS</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>4-User Acceptance</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>1-High</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>3-Big</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>005_SHOP_B2C_DSL_aktivuj_dsl_+_security_na_b2c_pres_shop</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>Proved kontrolu notifikaci SMS/Email</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>SMS/Email odpovida sablone</t>
         </is>
       </c>
     </row>

</xml_diff>